<commit_message>
switch to datannur name
</commit_message>
<xml_diff>
--- a/public/data/db_source/config.xlsx
+++ b/public/data/db_source/config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10714"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannuaire/datannuaire_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{759BFCB2-6BBD-3A48-B8CD-10D75C1CBE36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D8776C-0D84-C043-8A95-0D227C3371B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3220" yWindow="500" windowWidth="25580" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,9 +47,6 @@
     <t>contact_email</t>
   </si>
   <si>
-    <t>dat@nnuaire.email</t>
-  </si>
-  <si>
     <t>about_main</t>
   </si>
   <si>
@@ -103,15 +100,6 @@
   </si>
   <si>
     <t>about_page_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">### Fonctionnement
-Datannuaire contient 7 entités principales. On peut les diviser en deux catégories, partie intérieur et partie extérieur aux datasets. Le **dataset** représente une table de base de données ou un fichier de données (excel, csv, ...) sous forme de tableau (lignes et colonnes).
-mermaid( 
-  $dataset -.-&gt; intérieur
-  $dataset -.-&gt; extérieur
-);
-</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -136,29 +124,6 @@
   </si>
   <si>
     <t>about_page_5</t>
-  </si>
-  <si>
-    <t>La vue Meta représente les méta-méta-données, c’est-à-dire l'information sur les jeux de données internes au catalogue. 
-Cette vue apporte une synthèse générale sur le contenu du catalogue et permet de voir l'architecture de données de Datannuaire.
-Pour vérifier l'intégriter de la base de données, cliquez sur ce [lien](#!?app_mode=check_db).</t>
-  </si>
-  <si>
-    <t>![main_banner not_rounded](data/img/main_banner{dark_mode}.png?v=1)
-# datannuaire, le catalogue de données portable
-Permet de **centraliser**, **rechercher** et **visualiser** les informations sur une collection de jeux de données
-Pour améliorer l’organisation des données et faciliter leur **partage** et leur **documentation**
-**Simple** et **flexible**, s’intègre rapidement dans tous types d’environnement
-- **Facile** :
-Aucune installation ou configuration nécessaire, aucun coût ou prérequis technique
-- **Portable** :
-Fonctionne partout (local, cloud, disque partagé), un simple dossier que l’on peut copier, déplacer, envoyer et ouvrir avec n’importe quel navigateur web
-- **Complet** :
-Flexible, complet et structuré autour de 6 concepts avec un niveau de détail important : Institution, Dossier, Mot clé, Dataset, Variable et Modalité
-- **Indépendant** :
-Le catalogue n’est qu’une interface pour visualiser les métadonnées, le processus de leur création et mise à jour est indépendant et sous votre contrôle
-- **Sécurisé** :
-De pars la séparation stricte entre les deux systèmes, l’application est isolée dans le navigateur, ne peut rien modifier sur la machine et ne pose ainsi aucun risque
-La version ici présente est un **prototype** en cours de développement et d'expérimentation. Les données utilisées sont fictives et uniquement à usage de test et de développement. Question ou suggestion : [dat@nnuaire.email](mailto:dat@nnuaire.email).</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -227,6 +192,41 @@
   </si>
   <si>
     <t>Certaines entités possèdent des docs (documents de type markdown ou pdf). Un **doc** peut être lié à une multitude de datasets, de dossiers et d'institutions, et inversement.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">### Fonctionnement
+datannur contient 7 entités principales. On peut les diviser en deux catégories, partie intérieur et partie extérieur aux datasets. Le **dataset** représente une table de base de données ou un fichier de données (excel, csv, ...) sous forme de tableau (lignes et colonnes).
+mermaid( 
+  $dataset -.-&gt; intérieur
+  $dataset -.-&gt; extérieur
+);
+</t>
+  </si>
+  <si>
+    <t>contact@datannur.com</t>
+  </si>
+  <si>
+    <t>![main_banner not_rounded](data/img/main_banner{dark_mode}.png?v=1)
+# datannur, le catalogue de données portable
+Permet de **centraliser**, **rechercher** et **visualiser** les informations sur une collection de jeux de données
+Pour améliorer l’organisation des données et faciliter leur **partage** et leur **documentation**
+**Simple** et **flexible**, s’intègre rapidement dans tous types d’environnement
+- **Facile** :
+Aucune installation ou configuration nécessaire, aucun coût ou prérequis technique
+- **Portable** :
+Fonctionne partout (local, cloud, disque partagé), un simple dossier que l’on peut copier, déplacer, envoyer et ouvrir avec n’importe quel navigateur web
+- **Complet** :
+Flexible, complet et structuré autour de 6 concepts avec un niveau de détail important : Institution, Dossier, Mot clé, Dataset, Variable et Modalité
+- **Indépendant** :
+Le catalogue n’est qu’une interface pour visualiser les métadonnées, le processus de leur création et mise à jour est indépendant et sous votre contrôle
+- **Sécurisé** :
+De pars la séparation stricte entre les deux systèmes, l’application est isolée dans le navigateur, ne peut rien modifier sur la machine et ne pose ainsi aucun risque
+La version ici présente est un **prototype** en cours de développement et d'expérimentation. Les données utilisées sont fictives et uniquement à usage de test et de développement. Question ou suggestion : [contact@datannur.com](mailto:contact@datannur.com).</t>
+  </si>
+  <si>
+    <t>La vue méta représente les méta-méta-données, c’est-à-dire l'information sur les jeux de données internes au catalogue. 
+Cette vue apporte une synthèse générale sur le contenu du catalogue et permet de voir l'architecture de données de datannur.
+Pour vérifier l'intégriter de la base de données, cliquez sur ce [lien](?app_mode=check_db).</t>
   </si>
 </sst>
 </file>
@@ -289,7 +289,6 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -299,6 +298,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -653,10 +653,10 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -677,142 +677,142 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
+      <c r="B2" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>28</v>
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="170" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="289" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>29</v>
+        <v>18</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="136" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>33</v>
+        <v>19</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="404" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>32</v>
+        <v>24</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="119" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>27</v>
+        <v>4</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>12</v>
+        <v>5</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>31</v>
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>30</v>
+        <v>8</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>15</v>
+        <v>23</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{661DA68A-C646-1748-9C7C-4A5B6C0029BE}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{13CF6642-6EED-DC46-BFA2-86518A2CB838}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
add dependencies license info in readme
</commit_message>
<xml_diff>
--- a/public/data/db_source/config.xlsx
+++ b/public/data/db_source/config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannuaire/datannuaire_dev/public/data/db_source/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D8776C-0D84-C043-8A95-0D227C3371B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332447E3-68EE-1745-A025-6938BDC6DFD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3220" yWindow="500" windowWidth="25580" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -156,8 +156,54 @@
     <t>Les mots clés, ou tags, peuvent être attribués aux variables, aux datasets, aux institutions et aux dossiers.</t>
   </si>
   <si>
+    <t>about_doc</t>
+  </si>
+  <si>
+    <t>contact@datannur.com</t>
+  </si>
+  <si>
+    <t>La vue méta représente les méta-méta-données, c’est-à-dire l'information sur les jeux de données internes au catalogue. 
+Cette vue apporte une synthèse générale sur le contenu du catalogue et permet de voir l'architecture de données de datannur.
+Pour vérifier l'intégriter de la base de données, cliquez sur ce [lien](?app_mode=check_db).</t>
+  </si>
+  <si>
+    <t>![main_banner not_rounded](data/img/main_banner{dark_mode}.png?v=1)
+# datannur, le catalogue de données portable
+Permet de **centraliser**, **rechercher** et **visualiser** les informations sur une collection de jeux de données
+Pour améliorer l’organisation des données et faciliter leur **partage** et leur **documentation**
+**Simple** et **flexible**, s’intègre rapidement dans tous types d’environnement
+- **Facile** :
+Aucune installation ou configuration nécessaire, aucun coût ou prérequis technique
+- **Portable** :
+Fonctionne partout (local, cloud, disque partagé), un simple dossier que l’on peut copier, déplacer, envoyer et ouvrir avec n’importe quel navigateur web
+- **Complet** :
+Flexible, complet et structuré autour de 7 concepts avec un niveau de détail important : Institution, Dossier, Mot clé, Dataset, Variable et Modalité
+- **Indépendant** :
+Le catalogue n’est qu’une interface pour visualiser les métadonnées, le processus de leur création et mise à jour est indépendant et sous votre contrôle
+- **Sécurisé** :
+De pars la séparation stricte entre les deux systèmes, l’application est isolée dans le navigateur, ne peut rien modifier sur la machine et ne pose ainsi aucun risque
+La version ici présente est un **prototype** en cours de développement et d'expérimentation. Les données utilisées sont fictives et uniquement à usage de test et de développement. Question ou suggestion : [contact@datannur.com](mailto:contact@datannur.com).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">### Fonctionnement
+datannur contient 7 concepts principaux. On peut les diviser en deux catégories, partie intérieur et partie extérieur aux datasets. Le **dataset** représente une table de base de données ou un fichier de données (excel, csv, ...) sous forme de tableau (lignes et colonnes).
+mermaid( 
+  $dataset -.-&gt; intérieur
+  $dataset -.-&gt; extérieur
+);
+</t>
+  </si>
+  <si>
+    <t>Pour finir, certains concepts possèdent des docs (documents de type markdown ou pdf). Un **doc** peut être lié à une multitude de datasets, de dossiers et d'institutions, et inversement.
+mermaid(
+  $doc &lt;--&gt; $institution
+  $doc &lt;--&gt; $folder
+  $doc &lt;--&gt; $dataset
+);</t>
+  </si>
+  <si>
     <t xml:space="preserve">#### Vision d'ensemble
-Voici les liens entre les 7 entités, à l'intérieur et l'extérieur des datasets.
+Voici les liens entre les 7 concepts, à l'intérieur et l'extérieur des datasets.
 mermaid(
   $folder $recursive
   $institution $recursive
@@ -180,53 +226,7 @@
 </t>
   </si>
   <si>
-    <t>Pour finir, certaines entités possèdent des docs (documents de type markdown ou pdf). Un **doc** peut être lié à une multitude de datasets, de dossiers et d'institutions, et inversement.
-mermaid(
-  $doc &lt;--&gt; $institution
-  $doc &lt;--&gt; $folder
-  $doc &lt;--&gt; $dataset
-);</t>
-  </si>
-  <si>
-    <t>about_doc</t>
-  </si>
-  <si>
-    <t>Certaines entités possèdent des docs (documents de type markdown ou pdf). Un **doc** peut être lié à une multitude de datasets, de dossiers et d'institutions, et inversement.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">### Fonctionnement
-datannur contient 7 entités principales. On peut les diviser en deux catégories, partie intérieur et partie extérieur aux datasets. Le **dataset** représente une table de base de données ou un fichier de données (excel, csv, ...) sous forme de tableau (lignes et colonnes).
-mermaid( 
-  $dataset -.-&gt; intérieur
-  $dataset -.-&gt; extérieur
-);
-</t>
-  </si>
-  <si>
-    <t>contact@datannur.com</t>
-  </si>
-  <si>
-    <t>![main_banner not_rounded](data/img/main_banner{dark_mode}.png?v=1)
-# datannur, le catalogue de données portable
-Permet de **centraliser**, **rechercher** et **visualiser** les informations sur une collection de jeux de données
-Pour améliorer l’organisation des données et faciliter leur **partage** et leur **documentation**
-**Simple** et **flexible**, s’intègre rapidement dans tous types d’environnement
-- **Facile** :
-Aucune installation ou configuration nécessaire, aucun coût ou prérequis technique
-- **Portable** :
-Fonctionne partout (local, cloud, disque partagé), un simple dossier que l’on peut copier, déplacer, envoyer et ouvrir avec n’importe quel navigateur web
-- **Complet** :
-Flexible, complet et structuré autour de 6 concepts avec un niveau de détail important : Institution, Dossier, Mot clé, Dataset, Variable et Modalité
-- **Indépendant** :
-Le catalogue n’est qu’une interface pour visualiser les métadonnées, le processus de leur création et mise à jour est indépendant et sous votre contrôle
-- **Sécurisé** :
-De pars la séparation stricte entre les deux systèmes, l’application est isolée dans le navigateur, ne peut rien modifier sur la machine et ne pose ainsi aucun risque
-La version ici présente est un **prototype** en cours de développement et d'expérimentation. Les données utilisées sont fictives et uniquement à usage de test et de développement. Question ou suggestion : [contact@datannur.com](mailto:contact@datannur.com).</t>
-  </si>
-  <si>
-    <t>La vue méta représente les méta-méta-données, c’est-à-dire l'information sur les jeux de données internes au catalogue. 
-Cette vue apporte une synthèse générale sur le contenu du catalogue et permet de voir l'architecture de données de datannur.
-Pour vérifier l'intégriter de la base de données, cliquez sur ce [lien](?app_mode=check_db).</t>
+    <t>Certains concepts possèdent des docs (documents de type markdown ou pdf). Un **doc** peut être lié à une multitude de datasets, de dossiers et d'institutions, et inversement.</t>
   </si>
 </sst>
 </file>
@@ -653,10 +653,10 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -678,7 +678,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
@@ -686,7 +686,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="170" x14ac:dyDescent="0.2">
@@ -718,7 +718,7 @@
         <v>19</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="404" x14ac:dyDescent="0.2">
@@ -726,7 +726,7 @@
         <v>24</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="119" x14ac:dyDescent="0.2">
@@ -734,7 +734,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="34" x14ac:dyDescent="0.2">
@@ -803,10 +803,10 @@
     </row>
     <row r="18" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add changelog, highlight md links, update config about_main
</commit_message>
<xml_diff>
--- a/public/data/db_source/config.xlsx
+++ b/public/data/db_source/config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10811"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332447E3-68EE-1745-A025-6938BDC6DFD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A56080-87F0-A34B-A21D-E1BA37D48D9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3220" yWindow="500" windowWidth="25580" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -167,24 +167,6 @@
 Pour vérifier l'intégriter de la base de données, cliquez sur ce [lien](?app_mode=check_db).</t>
   </si>
   <si>
-    <t>![main_banner not_rounded](data/img/main_banner{dark_mode}.png?v=1)
-# datannur, le catalogue de données portable
-Permet de **centraliser**, **rechercher** et **visualiser** les informations sur une collection de jeux de données
-Pour améliorer l’organisation des données et faciliter leur **partage** et leur **documentation**
-**Simple** et **flexible**, s’intègre rapidement dans tous types d’environnement
-- **Facile** :
-Aucune installation ou configuration nécessaire, aucun coût ou prérequis technique
-- **Portable** :
-Fonctionne partout (local, cloud, disque partagé), un simple dossier que l’on peut copier, déplacer, envoyer et ouvrir avec n’importe quel navigateur web
-- **Complet** :
-Flexible, complet et structuré autour de 7 concepts avec un niveau de détail important : Institution, Dossier, Mot clé, Dataset, Variable et Modalité
-- **Indépendant** :
-Le catalogue n’est qu’une interface pour visualiser les métadonnées, le processus de leur création et mise à jour est indépendant et sous votre contrôle
-- **Sécurisé** :
-De pars la séparation stricte entre les deux systèmes, l’application est isolée dans le navigateur, ne peut rien modifier sur la machine et ne pose ainsi aucun risque
-La version ici présente est un **prototype** en cours de développement et d'expérimentation. Les données utilisées sont fictives et uniquement à usage de test et de développement. Question ou suggestion : [contact@datannur.com](mailto:contact@datannur.com).</t>
-  </si>
-  <si>
     <t xml:space="preserve">### Fonctionnement
 datannur contient 7 concepts principaux. On peut les diviser en deux catégories, partie intérieur et partie extérieur aux datasets. Le **dataset** représente une table de base de données ou un fichier de données (excel, csv, ...) sous forme de tableau (lignes et colonnes).
 mermaid( 
@@ -227,6 +209,23 @@
   </si>
   <si>
     <t>Certains concepts possèdent des docs (documents de type markdown ou pdf). Un **doc** peut être lié à une multitude de datasets, de dossiers et d'institutions, et inversement.</t>
+  </si>
+  <si>
+    <t>![main_banner not_rounded](data/img/main_banner{dark_mode}.png?v=1)
+# datannur, le catalogue de données portable
+Permet de centraliser, rechercher et visualiser les informations sur une collection de jeux de données
+Pour améliorer l’organisation des données et faciliter leur partage et leur documentation
+Simple et flexible, s’intègre rapidement dans tous types d’environnement
+- **Facile** :
+Aucune installation ou configuration nécessaire. datannur est le catalogue le plus simple à implémenter et maintenir
+- **Portable** :
+Fonctionne partout (local, cloud, disque partagé), un dossier que l’on peut copier, déplacer, envoyer et ouvrir avec n’importe quel navigateur
+- **Complet** :
+Flexible, complet et structuré autour de 7 concepts avec un niveau de détail important : Institution, Dossier, Mot clé, Doc, Dataset, Variable et Modalité
+- **Sécurisé** :
+Parce qu’elle est une simple interface HTML isolée dans le navigateur, l’application ne peut rien modifier sur la machine et ne pose ainsi aucun risque
+Pour davantage d'information : [datannur.com](https://datannur.com)
+La version ici présente est un prototype en cours de développement et d'expérimentation. Les données utilisées sont fictives et uniquement à usage de test et de développement. Question ou suggestion : [contact@datannur.com](mailto:contact@datannur.com).</t>
   </si>
 </sst>
 </file>
@@ -656,7 +655,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -686,7 +685,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="170" x14ac:dyDescent="0.2">
@@ -694,7 +693,7 @@
         <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="289" x14ac:dyDescent="0.2">
@@ -718,7 +717,7 @@
         <v>19</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="404" x14ac:dyDescent="0.2">
@@ -726,7 +725,7 @@
         <v>24</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="119" x14ac:dyDescent="0.2">
@@ -806,7 +805,7 @@
         <v>28</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed typo in about page, fixed tab title initial width too large on static page
</commit_message>
<xml_diff>
--- a/public/data/db_source/config.xlsx
+++ b/public/data/db_source/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A56080-87F0-A34B-A21D-E1BA37D48D9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D88D2CD-CFDD-A343-A2E4-14C8724E44EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3220" yWindow="500" windowWidth="25580" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -102,17 +102,6 @@
     <t>about_page_4</t>
   </si>
   <si>
-    <t xml:space="preserve">
-#### Intérieur du dataset
-Un dataset contient des variables (colonnes du tableau ou attributs de la table). Une **variable** est une liste de valeurs qui varient en fonction des individus ou ligne du tableau.
-mermaid( $dataset --&gt; $variable );
-Certaines variables sont de type catégoriel et peuvent être liées à une modalité, c'est à dire un ensemble de valeurs possibles. Une même **modalité** peut être liée à plusieurs variables de différents datasets. Une même variable peut être liée à plusieurs modalités.
-mermaid( $variable &lt;--&gt; $modality );
-Une modalité contient des valeurs possibles. Une **valeur** comprend optionnellement une description. 
-mermaid($modality --&gt; $value );
-</t>
-  </si>
-  <si>
     <t>about_institution</t>
   </si>
   <si>
@@ -124,30 +113,6 @@
   </si>
   <si>
     <t>about_page_5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-#### Extérieur du dataset
-Un dataset ou une modalité peut être contenu dans un dossier. Un **dossier** peut lui aussi être contenu dans un autre dossier et ainsi de suite, formant ainsi une arborescence.
-mermaid(
-  $folder $recursive
-  $folder --&gt; $dataset
-  $folder --&gt; $modality
-);
-Un dataset ou un dossier peut avoir un fournisseur et un gestionnaire. Il s'agit de deux rôles incarnés par une institution. Une **institution** peut être contenue dans une autre institution et ainsi de suite, de façon similaire aux dossiers.
-mermaid(
-  $institution $recursive
-  $institution -- manager - owner --&gt; $folder
-  $institution -- manager - owner --&gt; $dataset
-);
-Un dataset, un dossier ou une institution peuvent être lié à un ou plusieurs mots clés. Un **mot clé** peut être lié à une multitude de variables, de datasets, de dossiers et d'institutions. Un **mot clé** peut être contenue dans un autre mot clé et ainsi de suite, de façon similaire aux dossiers et aux institutions.
-mermaid(
-  $tag $recursive
-  $tag &lt;--&gt; $institution
-  $tag &lt;--&gt; $folder
-  $tag &lt;--&gt; $dataset
-  $tag &lt;--&gt; $variable
-);</t>
   </si>
   <si>
     <t>Les variables sont spécifiques à un dataset. Elles peuvent être liées à une ou plusieurs modalités.Des mots clés peuvent lui être attribué.</t>
@@ -215,7 +180,7 @@
 # datannur, le catalogue de données portable
 Permet de centraliser, rechercher et visualiser les informations sur une collection de jeux de données
 Pour améliorer l’organisation des données et faciliter leur partage et leur documentation
-Simple et flexible, s’intègre rapidement dans tous types d’environnement
+Simple et flexible, s’intègre rapidement dans tous types d’environnements
 - **Facile** :
 Aucune installation ou configuration nécessaire. datannur est le catalogue le plus simple à implémenter et maintenir
 - **Portable** :
@@ -226,6 +191,41 @@
 Parce qu’elle est une simple interface HTML isolée dans le navigateur, l’application ne peut rien modifier sur la machine et ne pose ainsi aucun risque
 Pour davantage d'information : [datannur.com](https://datannur.com)
 La version ici présente est un prototype en cours de développement et d'expérimentation. Les données utilisées sont fictives et uniquement à usage de test et de développement. Question ou suggestion : [contact@datannur.com](mailto:contact@datannur.com).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+#### Intérieur du dataset
+Un dataset contient des variables (colonnes du tableau ou attributs de la table). Une **variable** est une liste de valeurs qui varie en fonction des individus ou lignes du tableau.
+mermaid( $dataset --&gt; $variable );
+Certaines variables sont de type catégoriel et peuvent être liées à une modalité, c'est à dire un ensemble de valeurs possibles. Une même **modalité** peut être liée à plusieurs variables de différents datasets. Une même variable peut être liée à plusieurs modalités.
+mermaid( $variable &lt;--&gt; $modality );
+Une modalité contient des valeurs possibles. Une **valeur** comprend optionnellement une description. 
+mermaid($modality --&gt; $value );
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+#### Extérieur du dataset
+Un dataset ou une modalité peut être contenu dans un dossier. Un **dossier** peut lui aussi être contenu dans un autre dossier et ainsi de suite, formant ainsi une arborescence.
+mermaid(
+  $folder $recursive
+  $folder --&gt; $dataset
+  $folder --&gt; $modality
+);
+Un dataset ou un dossier peut avoir un fournisseur et un gestionnaire. Il s'agit de deux rôles incarnés par une institution. Une **institution** peut être contenue dans une autre institution et ainsi de suite, de façon similaire aux dossiers.
+mermaid(
+  $institution $recursive
+  $institution -- manager - owner --&gt; $folder
+  $institution -- manager - owner --&gt; $dataset
+);
+Un dataset, un dossier ou une institution peuvent être liés à un ou plusieurs mots clés. Un **mot clé** peut être lié à une multitude de variables, de datasets, de dossiers et d'institutions. Un **mot clé** peut être contenu dans un autre mot clé et ainsi de suite, de façon similaire aux dossiers et aux institutions.
+mermaid(
+  $tag $recursive
+  $tag &lt;--&gt; $institution
+  $tag &lt;--&gt; $folder
+  $tag &lt;--&gt; $dataset
+  $tag &lt;--&gt; $variable
+);</t>
   </si>
 </sst>
 </file>
@@ -652,10 +652,10 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -677,7 +677,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
@@ -685,7 +685,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="170" x14ac:dyDescent="0.2">
@@ -693,7 +693,7 @@
         <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="289" x14ac:dyDescent="0.2">
@@ -701,7 +701,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
@@ -709,7 +709,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="136" x14ac:dyDescent="0.2">
@@ -717,15 +717,15 @@
         <v>19</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="404" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="119" x14ac:dyDescent="0.2">
@@ -733,15 +733,15 @@
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="34" x14ac:dyDescent="0.2">
@@ -757,7 +757,7 @@
         <v>6</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="51" x14ac:dyDescent="0.2">
@@ -773,7 +773,7 @@
         <v>8</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="34" x14ac:dyDescent="0.2">
@@ -794,7 +794,7 @@
     </row>
     <row r="17" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>14</v>
@@ -802,10 +802,10 @@
     </row>
     <row r="18" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed : use internal markdown files instead of config.xlsx for about tab
</commit_message>
<xml_diff>
--- a/public/data/db_source/config.xlsx
+++ b/public/data/db_source/config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10908"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D88D2CD-CFDD-A343-A2E4-14C8724E44EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D6DC18-27DE-CE45-B88E-44E6791F2BEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3220" yWindow="500" windowWidth="25580" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>id</t>
   </si>
@@ -50,130 +50,7 @@
     <t>about_main</t>
   </si>
   <si>
-    <t>about_main_meta</t>
-  </si>
-  <si>
-    <t>about_folder</t>
-  </si>
-  <si>
-    <t>about_tag</t>
-  </si>
-  <si>
-    <t>about_dataset</t>
-  </si>
-  <si>
-    <t>about_variable</t>
-  </si>
-  <si>
-    <t>about_favorite</t>
-  </si>
-  <si>
-    <t>Le dataset est l'élément central du catalogue.
-Il contient un certain nombre de variable, il peut est membre d'un dossier et peut être géré par une institution. 
-Des mots clés peuvent lui être attribué.</t>
-  </si>
-  <si>
-    <t>Les dossiers permettent de regrouper et organiser les jeux de données en une arborescence. Un dossier peut être indiqué comme étant géré par une institution, et des mots clés peuvent lui être attribué.</t>
-  </si>
-  <si>
-    <t>about_modality</t>
-  </si>
-  <si>
-    <t>Une modalité comprend un ensemble de valeurs possibles pour une variable. 
-Elle peut être utilisée par une multitude de variable de différents datasets.</t>
-  </si>
-  <si>
-    <t>Cette page regroupe les options et les logs d'utilisation du catalogue. Les logs sont enregistrés dans le navigateur web.</t>
-  </si>
-  <si>
-    <t>Tous les éléments du catalogue peuvent être mis en favoris en cliquant sur **l'étoile**. 
-C'est sur cette page que tous les éléments favoris sont rassemblés. Les favoris sont enregistrés dans le navigateur web.</t>
-  </si>
-  <si>
-    <t>about_page_1</t>
-  </si>
-  <si>
-    <t>about_page_2</t>
-  </si>
-  <si>
-    <t>about_page_3</t>
-  </si>
-  <si>
-    <t>about_page_4</t>
-  </si>
-  <si>
-    <t>about_institution</t>
-  </si>
-  <si>
-    <t>Les institutions sont fournisseur et/ou gestionnaires de jeux de données et de dossiers.
-Elles sont regroupées en une arborescence pouvant aller jusqu'aux collaborateurs.</t>
-  </si>
-  <si>
-    <t>about_options</t>
-  </si>
-  <si>
-    <t>about_page_5</t>
-  </si>
-  <si>
-    <t>Les variables sont spécifiques à un dataset. Elles peuvent être liées à une ou plusieurs modalités.Des mots clés peuvent lui être attribué.</t>
-  </si>
-  <si>
-    <t>Les mots clés, ou tags, peuvent être attribués aux variables, aux datasets, aux institutions et aux dossiers.</t>
-  </si>
-  <si>
-    <t>about_doc</t>
-  </si>
-  <si>
     <t>contact@datannur.com</t>
-  </si>
-  <si>
-    <t>La vue méta représente les méta-méta-données, c’est-à-dire l'information sur les jeux de données internes au catalogue. 
-Cette vue apporte une synthèse générale sur le contenu du catalogue et permet de voir l'architecture de données de datannur.
-Pour vérifier l'intégriter de la base de données, cliquez sur ce [lien](?app_mode=check_db).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">### Fonctionnement
-datannur contient 7 concepts principaux. On peut les diviser en deux catégories, partie intérieur et partie extérieur aux datasets. Le **dataset** représente une table de base de données ou un fichier de données (excel, csv, ...) sous forme de tableau (lignes et colonnes).
-mermaid( 
-  $dataset -.-&gt; intérieur
-  $dataset -.-&gt; extérieur
-);
-</t>
-  </si>
-  <si>
-    <t>Pour finir, certains concepts possèdent des docs (documents de type markdown ou pdf). Un **doc** peut être lié à une multitude de datasets, de dossiers et d'institutions, et inversement.
-mermaid(
-  $doc &lt;--&gt; $institution
-  $doc &lt;--&gt; $folder
-  $doc &lt;--&gt; $dataset
-);</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#### Vision d'ensemble
-Voici les liens entre les 7 concepts, à l'intérieur et l'extérieur des datasets.
-mermaid(
-  $folder $recursive
-  $institution $recursive
-  $tag $recursive
-  $institution -- manager - owner --&gt; $dataset
-  $institution -- manager - owner --&gt; $folder
-  $folder --&gt; $dataset
-  $folder --&gt; $modality
-  $tag &lt;--&gt; $institution
-  $tag &lt;--&gt; $folder
-  $tag &lt;--&gt; $dataset
-  $tag &lt;--&gt; $variable
-  $doc &lt;--&gt; $institution
-  $doc &lt;--&gt; $folder
-  $doc &lt;--&gt; $dataset
-  $dataset --&gt; $variable
-  $variable &lt;--&gt; $modality
-  $modality --&gt; $value
-  );
-</t>
-  </si>
-  <si>
-    <t>Certains concepts possèdent des docs (documents de type markdown ou pdf). Un **doc** peut être lié à une multitude de datasets, de dossiers et d'institutions, et inversement.</t>
   </si>
   <si>
     <t>![main_banner not_rounded](data/img/main_banner{dark_mode}.png?v=1)
@@ -192,47 +69,12 @@
 Pour davantage d'information : [datannur.com](https://datannur.com)
 La version ici présente est un prototype en cours de développement et d'expérimentation. Les données utilisées sont fictives et uniquement à usage de test et de développement. Question ou suggestion : [contact@datannur.com](mailto:contact@datannur.com).</t>
   </si>
-  <si>
-    <t xml:space="preserve">
-#### Intérieur du dataset
-Un dataset contient des variables (colonnes du tableau ou attributs de la table). Une **variable** est une liste de valeurs qui varie en fonction des individus ou lignes du tableau.
-mermaid( $dataset --&gt; $variable );
-Certaines variables sont de type catégoriel et peuvent être liées à une modalité, c'est à dire un ensemble de valeurs possibles. Une même **modalité** peut être liée à plusieurs variables de différents datasets. Une même variable peut être liée à plusieurs modalités.
-mermaid( $variable &lt;--&gt; $modality );
-Une modalité contient des valeurs possibles. Une **valeur** comprend optionnellement une description. 
-mermaid($modality --&gt; $value );
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-#### Extérieur du dataset
-Un dataset ou une modalité peut être contenu dans un dossier. Un **dossier** peut lui aussi être contenu dans un autre dossier et ainsi de suite, formant ainsi une arborescence.
-mermaid(
-  $folder $recursive
-  $folder --&gt; $dataset
-  $folder --&gt; $modality
-);
-Un dataset ou un dossier peut avoir un fournisseur et un gestionnaire. Il s'agit de deux rôles incarnés par une institution. Une **institution** peut être contenue dans une autre institution et ainsi de suite, de façon similaire aux dossiers.
-mermaid(
-  $institution $recursive
-  $institution -- manager - owner --&gt; $folder
-  $institution -- manager - owner --&gt; $dataset
-);
-Un dataset, un dossier ou une institution peuvent être liés à un ou plusieurs mots clés. Un **mot clé** peut être lié à une multitude de variables, de datasets, de dossiers et d'institutions. Un **mot clé** peut être contenu dans un autre mot clé et ainsi de suite, de façon similaire aux dossiers et aux institutions.
-mermaid(
-  $tag $recursive
-  $tag &lt;--&gt; $institution
-  $tag &lt;--&gt; $folder
-  $tag &lt;--&gt; $dataset
-  $tag &lt;--&gt; $variable
-);</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -247,16 +89,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri (Corps)"/>
     </font>
     <font>
       <sz val="8"/>
@@ -286,15 +118,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -317,8 +143,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9BB74F48-D0F4-FA4B-A818-58266F20AB52}" name="Tableau1" displayName="Tableau1" ref="A1:B18" totalsRowShown="0">
-  <autoFilter ref="A1:B18" xr:uid="{9BB74F48-D0F4-FA4B-A818-58266F20AB52}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9BB74F48-D0F4-FA4B-A818-58266F20AB52}" name="Tableau1" displayName="Tableau1" ref="A1:B3" totalsRowShown="0">
+  <autoFilter ref="A1:B3" xr:uid="{9BB74F48-D0F4-FA4B-A818-58266F20AB52}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{A513F0B6-5730-454E-B160-F273AA355AF9}" name="id"/>
     <tableColumn id="3" xr3:uid="{C6F40ACF-8A8F-094A-9103-5E1A8AABEC96}" name="value" dataCellStyle="Lien hypertexte"/>
@@ -649,13 +475,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -676,8 +502,8 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>27</v>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
@@ -685,131 +511,11 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="170" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="289" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="136" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="404" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="119" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
         <v>5</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{13CF6642-6EED-DC46-BFA2-86518A2CB838}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
changed : make about_main internal markdown with optional custom parts
</commit_message>
<xml_diff>
--- a/public/data/db_source/config.xlsx
+++ b/public/data/db_source/config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10916"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D6DC18-27DE-CE45-B88E-44E6791F2BEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9856FFD1-4E6C-1B4C-8987-FF2BCA2D9D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3220" yWindow="500" windowWidth="25580" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>id</t>
   </si>
@@ -47,27 +47,7 @@
     <t>contact_email</t>
   </si>
   <si>
-    <t>about_main</t>
-  </si>
-  <si>
     <t>contact@datannur.com</t>
-  </si>
-  <si>
-    <t>![main_banner not_rounded](data/img/main_banner{dark_mode}.png?v=1)
-# datannur, le catalogue de données portable
-Permet de centraliser, rechercher et visualiser les informations sur une collection de jeux de données
-Pour améliorer l’organisation des données et faciliter leur partage et leur documentation
-Simple et flexible, s’intègre rapidement dans tous types d’environnements
-- **Facile** :
-Aucune installation ou configuration nécessaire. datannur est le catalogue le plus simple à implémenter et maintenir
-- **Portable** :
-Fonctionne partout (local, cloud, disque partagé), un dossier que l’on peut copier, déplacer, envoyer et ouvrir avec n’importe quel navigateur
-- **Complet** :
-Flexible, complet et structuré autour de 7 concepts avec un niveau de détail important : Institution, Dossier, Mot clé, Doc, Dataset, Variable et Modalité
-- **Sécurisé** :
-Parce qu’elle est une simple interface HTML isolée dans le navigateur, l’application ne peut rien modifier sur la machine et ne pose ainsi aucun risque
-Pour davantage d'information : [datannur.com](https://datannur.com)
-La version ici présente est un prototype en cours de développement et d'expérimentation. Les données utilisées sont fictives et uniquement à usage de test et de développement. Question ou suggestion : [contact@datannur.com](mailto:contact@datannur.com).</t>
   </si>
 </sst>
 </file>
@@ -118,11 +98,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -143,8 +120,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9BB74F48-D0F4-FA4B-A818-58266F20AB52}" name="Tableau1" displayName="Tableau1" ref="A1:B3" totalsRowShown="0">
-  <autoFilter ref="A1:B3" xr:uid="{9BB74F48-D0F4-FA4B-A818-58266F20AB52}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9BB74F48-D0F4-FA4B-A818-58266F20AB52}" name="Tableau1" displayName="Tableau1" ref="A1:B2" totalsRowShown="0">
+  <autoFilter ref="A1:B2" xr:uid="{9BB74F48-D0F4-FA4B-A818-58266F20AB52}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{A513F0B6-5730-454E-B160-F273AA355AF9}" name="id"/>
     <tableColumn id="3" xr3:uid="{C6F40ACF-8A8F-094A-9103-5E1A8AABEC96}" name="value" dataCellStyle="Lien hypertexte"/>
@@ -475,13 +452,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" zoomScale="140" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -502,16 +479,8 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed : get last modification timestamp directly from jsonjsdb instead of info file
</commit_message>
<xml_diff>
--- a/public/data/db_source/config.xlsx
+++ b/public/data/db_source/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11013"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9856FFD1-4E6C-1B4C-8987-FF2BCA2D9D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE64C19-D179-A54D-B629-214EF2482321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3220" yWindow="500" windowWidth="25580" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>id</t>
   </si>
@@ -48,13 +48,37 @@
   </si>
   <si>
     <t>contact@datannur.com</t>
+  </si>
+  <si>
+    <t>alias_1</t>
+  </si>
+  <si>
+    <t>alias_2</t>
+  </si>
+  <si>
+    <t>filter_1</t>
+  </si>
+  <si>
+    <t>filter_2</t>
+  </si>
+  <si>
+    <t>institution : owner</t>
+  </si>
+  <si>
+    <t>institution : manager</t>
+  </si>
+  <si>
+    <t>open_data : Open Data</t>
+  </si>
+  <si>
+    <t>closed_data : Closed Data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -72,6 +96,12 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -98,9 +128,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -120,8 +151,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9BB74F48-D0F4-FA4B-A818-58266F20AB52}" name="Tableau1" displayName="Tableau1" ref="A1:B2" totalsRowShown="0">
-  <autoFilter ref="A1:B2" xr:uid="{9BB74F48-D0F4-FA4B-A818-58266F20AB52}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9BB74F48-D0F4-FA4B-A818-58266F20AB52}" name="Tableau1" displayName="Tableau1" ref="A1:B6" totalsRowShown="0">
+  <autoFilter ref="A1:B6" xr:uid="{9BB74F48-D0F4-FA4B-A818-58266F20AB52}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{A513F0B6-5730-454E-B160-F273AA355AF9}" name="id"/>
     <tableColumn id="3" xr3:uid="{C6F40ACF-8A8F-094A-9103-5E1A8AABEC96}" name="value" dataCellStyle="Lien hypertexte"/>
@@ -452,19 +483,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="140" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="98.83203125" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -483,15 +511,44 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{13CF6642-6EED-DC46-BFA2-86518A2CB838}"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
change : internalize alias for institution
</commit_message>
<xml_diff>
--- a/public/data/db_source/config.xlsx
+++ b/public/data/db_source/config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE64C19-D179-A54D-B629-214EF2482321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67742504-95B6-2643-8A71-FFB14369FEBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>id</t>
   </si>
@@ -50,22 +50,10 @@
     <t>contact@datannur.com</t>
   </si>
   <si>
-    <t>alias_1</t>
-  </si>
-  <si>
-    <t>alias_2</t>
-  </si>
-  <si>
     <t>filter_1</t>
   </si>
   <si>
     <t>filter_2</t>
-  </si>
-  <si>
-    <t>institution : owner</t>
-  </si>
-  <si>
-    <t>institution : manager</t>
   </si>
   <si>
     <t>open_data : Open Data</t>
@@ -128,9 +116,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -151,8 +138,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9BB74F48-D0F4-FA4B-A818-58266F20AB52}" name="Tableau1" displayName="Tableau1" ref="A1:B6" totalsRowShown="0">
-  <autoFilter ref="A1:B6" xr:uid="{9BB74F48-D0F4-FA4B-A818-58266F20AB52}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9BB74F48-D0F4-FA4B-A818-58266F20AB52}" name="Tableau1" displayName="Tableau1" ref="A1:B4" totalsRowShown="0">
+  <autoFilter ref="A1:B4" xr:uid="{9BB74F48-D0F4-FA4B-A818-58266F20AB52}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{A513F0B6-5730-454E-B160-F273AA355AF9}" name="id"/>
     <tableColumn id="3" xr3:uid="{C6F40ACF-8A8F-094A-9103-5E1A8AABEC96}" name="value" dataCellStyle="Lien hypertexte"/>
@@ -483,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="140" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -507,7 +494,7 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -515,32 +502,16 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>